<commit_message>
MTU changed again and exit all added
</commit_message>
<xml_diff>
--- a/FAS Config HFC WIP.xlsx
+++ b/FAS Config HFC WIP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rojan\demoapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB95E539-3FF9-4107-B533-B3C9DCD4C4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3A930E-7060-4F2E-8B03-3B60510AF425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="1" xr2:uid="{4A2FBDB7-EACF-420D-B1E9-809952438E9B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="132">
   <si>
     <t>Port configuration</t>
   </si>
@@ -425,7 +425,10 @@
     <t xml:space="preserve">                to &lt;Second_FAS_SYSTEM_IP&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">            mtu 2000</t>
+    <t xml:space="preserve">            mtu 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    exit all</t>
   </si>
 </sst>
 </file>
@@ -1715,7 +1718,7 @@
   <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1798,7 +1801,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
encapsulation changed and encap type changed
</commit_message>
<xml_diff>
--- a/FAS Config HFC WIP.xlsx
+++ b/FAS Config HFC WIP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rojan\demoapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3A930E-7060-4F2E-8B03-3B60510AF425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F2DDAB-B878-45CF-9359-3FC212D4F80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="1" xr2:uid="{4A2FBDB7-EACF-420D-B1E9-809952438E9B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="133">
   <si>
     <t>Port configuration</t>
   </si>
@@ -429,6 +429,9 @@
   </si>
   <si>
     <t xml:space="preserve">    exit all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            encap-type fot1q</t>
   </si>
 </sst>
 </file>
@@ -1718,7 +1721,7 @@
   <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1751,12 +1754,12 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>